<commit_message>
codes fy23 new and reused funds
</commit_message>
<xml_diff>
--- a/ioc_source_updated23_AWM.xlsx
+++ b/ioc_source_updated23_AWM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures IGPA\Fiscal Futures FY2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348D973-8CD3-4C12-8BB6-5E7760D81ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B251D-8926-4606-BED4-D66483BBE2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="-16200" windowWidth="14400" windowHeight="14985" xr2:uid="{95DD0F56-1BF5-4636-A2E6-971DE42DAC47}"/>
+    <workbookView xWindow="8640" yWindow="0" windowWidth="14400" windowHeight="12960" xr2:uid="{95DD0F56-1BF5-4636-A2E6-971DE42DAC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -15045,7 +15045,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49EEBAE8-29F6-463B-9B2F-33AF9E80ABD6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49EEBAE8-29F6-463B-9B2F-33AF9E80ABD6}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K41" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
@@ -15651,8 +15651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2425"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>